<commit_message>
move actions to design
</commit_message>
<xml_diff>
--- a/aircraft_outputs.xlsx
+++ b/aircraft_outputs.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C39"/>
+  <dimension ref="A1:C38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -535,7 +535,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>8535</v>
+        <v>6000</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
@@ -747,7 +747,7 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>21093.50425273008</v>
+        <v>19235.93618374716</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
@@ -762,7 +762,7 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>67707.11367456056</v>
+        <v>85128.60044282374</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
@@ -777,7 +777,7 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>35189.60942183048</v>
+        <v>54568.66425907657</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
@@ -801,7 +801,7 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>1598.656536988379</v>
+        <v>1246.114006310022</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
@@ -816,7 +816,7 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>10749.72838332894</v>
+        <v>9694.815192239563</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
@@ -831,7 +831,7 @@
         </is>
       </c>
       <c r="B30" t="n">
-        <v>6243.32026452595</v>
+        <v>6160.906687053855</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
@@ -846,7 +846,7 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>1929.9998132356</v>
+        <v>1337.865595885331</v>
       </c>
       <c r="C31" t="inlineStr">
         <is>
@@ -861,7 +861,7 @@
         </is>
       </c>
       <c r="B32" t="n">
-        <v>101.7482430393286</v>
+        <v>77.37596008705309</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
@@ -876,7 +876,7 @@
         </is>
       </c>
       <c r="B33" t="n">
-        <v>470.0510116118821</v>
+        <v>389.5769267962468</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
@@ -900,7 +900,7 @@
         </is>
       </c>
       <c r="B36" t="n">
-        <v>10.1108299875289</v>
+        <v>10.01505877647578</v>
       </c>
       <c r="C36" t="inlineStr">
         <is>
@@ -915,7 +915,7 @@
         </is>
       </c>
       <c r="B37" t="n">
-        <v>11.15979058353563</v>
+        <v>10.82710767237309</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
@@ -923,10 +923,18 @@
         </is>
       </c>
     </row>
-    <row r="39">
-      <c r="A39" t="inlineStr">
-        <is>
-          <t>Class I weight estimation</t>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Stability margin</t>
+        </is>
+      </c>
+      <c r="B38" t="n">
+        <v>-6.540066047709018</v>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>m</t>
         </is>
       </c>
     </row>

</xml_diff>